<commit_message>
new folders for univpos
</commit_message>
<xml_diff>
--- a/limba/limba_meta.xlsx
+++ b/limba/limba_meta.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>N</t>
   </si>
@@ -51,6 +51,27 @@
   </si>
   <si>
     <t>tape1_side1_tale3</t>
+  </si>
+  <si>
+    <t>tape1_side1_tale4</t>
+  </si>
+  <si>
+    <t>tape1_side1_tale5</t>
+  </si>
+  <si>
+    <t>tape1_side1_tale6</t>
+  </si>
+  <si>
+    <t>tape1_side1_tale7</t>
+  </si>
+  <si>
+    <t>SONG</t>
+  </si>
+  <si>
+    <t>maybe several tales by the same speaker</t>
+  </si>
+  <si>
+    <t>song in the end</t>
   </si>
 </sst>
 </file>
@@ -381,7 +402,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,20 +475,65 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.16527777777777777</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.10277777777777779</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.33263888888888887</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.14930555555555555</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>